<commit_message>
Add more api test
</commit_message>
<xml_diff>
--- a/API-Test-Cases.xlsx
+++ b/API-Test-Cases.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp 640 G2\Downloads\open-cart-demo-online-shopping-main\open-cart-demo-online-shopping-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAPTOP\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47096B9-A3F1-445B-8EAF-E172E3D4B0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A3E85BE-1C51-4FD5-8288-922F3B317CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F506F1E7-1669-43D9-8551-1234B563D8BA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F506F1E7-1669-43D9-8551-1234B563D8BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="276">
   <si>
     <r>
       <t xml:space="preserve">Valid </t>
@@ -840,52 +841,28 @@
     <t>No payload</t>
   </si>
   <si>
-    <t>B-005</t>
-  </si>
-  <si>
     <t>Status: 405 Method Not Allowed. Body: {"responseCode": 405, "message": "This request method is not supported."}</t>
   </si>
   <si>
     <t>Request Method: POST</t>
   </si>
   <si>
-    <t>B-004</t>
-  </si>
-  <si>
     <t>Status: 200 OK. Body: {"responseCode": 200, "brands": [...]}</t>
   </si>
   <si>
     <t>No payload (GET request)</t>
   </si>
   <si>
-    <t>B-001</t>
-  </si>
-  <si>
     <t>Any sample JSON payload</t>
   </si>
   <si>
-    <t>P2-001</t>
-  </si>
-  <si>
-    <t>P-004</t>
-  </si>
-  <si>
-    <t>P-003</t>
-  </si>
-  <si>
     <t>Status: 200 OK. Each product includes required fields.</t>
   </si>
   <si>
     <t>Status: 200 OK. Each product includes keys: id, name, price, brand, category.</t>
   </si>
   <si>
-    <t>P-002</t>
-  </si>
-  <si>
     <t>Status: 200 OK. Body: {"responseCode": 200, "products": [...]}</t>
-  </si>
-  <si>
-    <t>P-001</t>
   </si>
   <si>
     <r>
@@ -1222,12 +1199,544 @@
 "Password":"nourhan123^^"
 }</t>
   </si>
+  <si>
+    <t>Successful search. Verify that product search returns correct items.</t>
+  </si>
+  <si>
+    <t>No payload
+Request Method: PUT</t>
+  </si>
+  <si>
+    <t>Status: 405 Method Not Allowed
+Body: {"responseCode": 405, "message": "This request method is not supported."}</t>
+  </si>
+  <si>
+    <t>Expected Result:
+Status: 200 OK
+Body: {"responseCode": 200, "products": [...]}</t>
+  </si>
+  <si>
+    <t>Expected Result:
+Status: 200 OK
+Response time ≤ 3000ms</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Missing parameter. Verify error when </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>search_product</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is not provided.</t>
+    </r>
+  </si>
+  <si>
+    <t>Expected Result:
+Status: 400 Bad Request
+Body:
+{
+  "responseCode": 400,
+  "message": "search_product parameter is required"
+}</t>
+  </si>
+  <si>
+    <t>Verify response time within 3 seconds for invalid request.</t>
+  </si>
+  <si>
+    <t>Expected Result:
+Status: 400 Bad Request
+Response time ≤ 3000ms</t>
+  </si>
+  <si>
+    <t>PUT /brands/list Successful/Valid: Verify updating of brands list is blocked.</t>
+  </si>
+  <si>
+    <t>Verify response time is within 3 seconds.C12:C13</t>
+  </si>
+  <si>
+    <t>Execution Status</t>
+  </si>
+  <si>
+    <t>A4-001</t>
+  </si>
+  <si>
+    <t>PUT /brandsList: Invalid Method Check. Verify updating brand list is blocked.</t>
+  </si>
+  <si>
+    <t>No payload. Request Method: PUT</t>
+  </si>
+  <si>
+    <t>A4-002</t>
+  </si>
+  <si>
+    <t>PUT /brandsList: Verify response time within 3 seconds.</t>
+  </si>
+  <si>
+    <t>Status: 405 Method Not Allowed. Response time ≤ 3000ms</t>
+  </si>
+  <si>
+    <t>A4-003</t>
+  </si>
+  <si>
+    <t>PUT /brandsList: Validate response structure for invalid method.</t>
+  </si>
+  <si>
+    <t>Status: 405. Body includes keys: responseCode, message</t>
+  </si>
+  <si>
+    <t>A5-001</t>
+  </si>
+  <si>
+    <t>POST /searchProduct: Successful search. Verify returning correct items.</t>
+  </si>
+  <si>
+    <t>{ "search_product": "iphone" }</t>
+  </si>
+  <si>
+    <t>A5-002</t>
+  </si>
+  <si>
+    <t>POST /searchProduct: Verify response time is within 3 seconds.</t>
+  </si>
+  <si>
+    <t>{ "search_product": "laptop" }</t>
+  </si>
+  <si>
+    <t>A5-003</t>
+  </si>
+  <si>
+    <t>POST /searchProduct: Verify empty search result for non-existing product.</t>
+  </si>
+  <si>
+    <t>{ "search_product": "unknown_item_123" }</t>
+  </si>
+  <si>
+    <t>Status: 200 OK. Body: {"responseCode": 200, "products": []}</t>
+  </si>
+  <si>
+    <t>A5-004</t>
+  </si>
+  <si>
+    <t>POST /searchProduct: Invalid Method Check (GET).</t>
+  </si>
+  <si>
+    <t>Request Method: GET</t>
+  </si>
+  <si>
+    <t>A5-005</t>
+  </si>
+  <si>
+    <t>POST /searchProduct: Verify response structure.</t>
+  </si>
+  <si>
+    <t>{ "search_product": "camera" }</t>
+  </si>
+  <si>
+    <t>Status: 200 OK. Body includes keys: responseCode, products</t>
+  </si>
+  <si>
+    <t>A6-001</t>
+  </si>
+  <si>
+    <t>POST /searchProduct: Missing parameter. Verify error when search_product is not provided.</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>Status: 400 Bad Request. Body: {"responseCode": 400, "message": "search_product parameter is required"}</t>
+  </si>
+  <si>
+    <t>A6-002</t>
+  </si>
+  <si>
+    <t>POST /searchProduct: Verify response time within 3 seconds for invalid request.</t>
+  </si>
+  <si>
+    <t>Status: 400 Bad Request. Response time ≤ 3000ms</t>
+  </si>
+  <si>
+    <t>A6-003</t>
+  </si>
+  <si>
+    <t>POST /searchProduct: Invalid datatype. search_product sent as number.</t>
+  </si>
+  <si>
+    <t>{ "search_product": 12345 }</t>
+  </si>
+  <si>
+    <t>Status: 400 Bad Request. Body: {"responseCode": 400, "message": "search_product must be a string"}</t>
+  </si>
+  <si>
+    <t>A6-004</t>
+  </si>
+  <si>
+    <t>A6-005</t>
+  </si>
+  <si>
+    <t>POST /searchProduct: Verify special characters handling.</t>
+  </si>
+  <si>
+    <t>{ "search_product": "@@@@" }</t>
+  </si>
+  <si>
+    <t>Status: 405 Method Not Allowed. Response time ~100–200ms</t>
+  </si>
+  <si>
+    <t>Status: 405. Body contains keys: responseCode, message</t>
+  </si>
+  <si>
+    <t>Status: 200 OK. Response time ~120–300ms</t>
+  </si>
+  <si>
+    <t>Status: 200 OK. Response includes responseCode and products keys</t>
+  </si>
+  <si>
+    <t>Status: 400 Bad Request. Response time ~80–150ms</t>
+  </si>
+  <si>
+    <t>API-1-1</t>
+  </si>
+  <si>
+    <t>API-1-2</t>
+  </si>
+  <si>
+    <t>API-1-3</t>
+  </si>
+  <si>
+    <t>API-1-4</t>
+  </si>
+  <si>
+    <t>API-2-1</t>
+  </si>
+  <si>
+    <t>API-3-1</t>
+  </si>
+  <si>
+    <t>API-3-2</t>
+  </si>
+  <si>
+    <t>API-3-3</t>
+  </si>
+  <si>
+    <t>Verify dashboard loads successfully</t>
+  </si>
+  <si>
+    <t>GET /admin/dashboard</t>
+  </si>
+  <si>
+    <t>200 OK, dashboard data returned</t>
+  </si>
+  <si>
+    <t>Dashboard loaded, metrics partially missing</t>
+  </si>
+  <si>
+    <t>Verify new order updates dashboard metrics</t>
+  </si>
+  <si>
+    <t>Trigger new order</t>
+  </si>
+  <si>
+    <t>200 OK, metrics updated</t>
+  </si>
+  <si>
+    <t>Metrics did not update immediately</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Verify total sales calculation accuracy</t>
+  </si>
+  <si>
+    <t>GET /admin/dashboard/sales</t>
+  </si>
+  <si>
+    <t>200 OK, correct totals</t>
+  </si>
+  <si>
+    <t>Sales total off by 2% under load</t>
+  </si>
+  <si>
+    <t>Verify total orders count updates correctly</t>
+  </si>
+  <si>
+    <t>GET /admin/dashboard/orders</t>
+  </si>
+  <si>
+    <t>200 OK, correct order count</t>
+  </si>
+  <si>
+    <t>Order count correct</t>
+  </si>
+  <si>
+    <t>Verify dashboard shows correct number of customers</t>
+  </si>
+  <si>
+    <t>GET /admin/dashboard/customers</t>
+  </si>
+  <si>
+    <t>200 OK, customer count matches DB</t>
+  </si>
+  <si>
+    <t>Customer count correct</t>
+  </si>
+  <si>
+    <t>Verify sales graph loads correctly</t>
+  </si>
+  <si>
+    <t>GET /admin/dashboard/graph/sales</t>
+  </si>
+  <si>
+    <t>200 OK, JSON graph data returned</t>
+  </si>
+  <si>
+    <t>Graph loaded</t>
+  </si>
+  <si>
+    <t>Verify orders graph loads correctly</t>
+  </si>
+  <si>
+    <t>GET /admin/dashboard/graph/orders</t>
+  </si>
+  <si>
+    <t>Orders graph missing last hour</t>
+  </si>
+  <si>
+    <t>Verify dashboard graph filters by date range</t>
+  </si>
+  <si>
+    <t>GET /admin/dashboard/graph?s=2025-01-01&amp;e=2025-01-31</t>
+  </si>
+  <si>
+    <t>200 OK, filtered graph returned</t>
+  </si>
+  <si>
+    <t>Graph filtered correctly</t>
+  </si>
+  <si>
+    <t>API-9-1</t>
+  </si>
+  <si>
+    <t>API-9-2</t>
+  </si>
+  <si>
+    <t>API-9-3</t>
+  </si>
+  <si>
+    <t>API-9-4</t>
+  </si>
+  <si>
+    <t>API-9-5</t>
+  </si>
+  <si>
+    <t>API-9-6</t>
+  </si>
+  <si>
+    <t>API-9-7</t>
+  </si>
+  <si>
+    <t>API-9-8</t>
+  </si>
+  <si>
+    <t>Create new product with valid data</t>
+  </si>
+  <si>
+    <t>POST /admin/products {"name":"Test Product","price":100,"quantity":10,"sku":"TP100"}</t>
+  </si>
+  <si>
+    <t>200 OK, product created</t>
+  </si>
+  <si>
+    <t>Product created</t>
+  </si>
+  <si>
+    <t>Fail creating product with missing required fields</t>
+  </si>
+  <si>
+    <t>POST /admin/products {"price":100,"quantity":10}</t>
+  </si>
+  <si>
+    <t>400 Bad Request, missing required field 'name'</t>
+  </si>
+  <si>
+    <t>Error returned</t>
+  </si>
+  <si>
+    <t>Edit existing product</t>
+  </si>
+  <si>
+    <t>PUT /admin/products/{id} {"name":"Updated Product"}</t>
+  </si>
+  <si>
+    <t>200 OK, product updated</t>
+  </si>
+  <si>
+    <t>Product updated</t>
+  </si>
+  <si>
+    <t>Delete product successfully</t>
+  </si>
+  <si>
+    <t>DELETE /admin/products/{id}</t>
+  </si>
+  <si>
+    <t>200 OK, product deleted</t>
+  </si>
+  <si>
+    <t>Product deleted</t>
+  </si>
+  <si>
+    <t>Fail deleting product with invalid ID</t>
+  </si>
+  <si>
+    <t>DELETE /admin/products/99999</t>
+  </si>
+  <si>
+    <t>404 Not Found, product not found</t>
+  </si>
+  <si>
+    <t>404 returned</t>
+  </si>
+  <si>
+    <t>Verify product list loads</t>
+  </si>
+  <si>
+    <t>GET /admin/products</t>
+  </si>
+  <si>
+    <t>200 OK, product list returned</t>
+  </si>
+  <si>
+    <t>Product list incomplete due to pagination issue</t>
+  </si>
+  <si>
+    <t>Verify product status toggle</t>
+  </si>
+  <si>
+    <t>PATCH /admin/products/{id}/status {"status":"Enabled"}</t>
+  </si>
+  <si>
+    <t>200 OK, status updated</t>
+  </si>
+  <si>
+    <t>Status toggle failed for one product</t>
+  </si>
+  <si>
+    <t>Search product by name</t>
+  </si>
+  <si>
+    <t>GET /admin/products?search=Test</t>
+  </si>
+  <si>
+    <t>200 OK, products match search query</t>
+  </si>
+  <si>
+    <t>Search results correct</t>
+  </si>
+  <si>
+    <t>Search product by SKU</t>
+  </si>
+  <si>
+    <t>GET /admin/products?sku=TP100</t>
+  </si>
+  <si>
+    <t>200 OK, correct product returned</t>
+  </si>
+  <si>
+    <t>Product returned</t>
+  </si>
+  <si>
+    <t>Filter products by category</t>
+  </si>
+  <si>
+    <t>GET /admin/products?category=Electronics</t>
+  </si>
+  <si>
+    <t>200 OK, products filtered by category</t>
+  </si>
+  <si>
+    <t>Products filtered correctly</t>
+  </si>
+  <si>
+    <t>Filter products by status</t>
+  </si>
+  <si>
+    <t>GET /admin/products?status=Enabled</t>
+  </si>
+  <si>
+    <t>200 OK, filtered products returned</t>
+  </si>
+  <si>
+    <t>Some disabled products appeared</t>
+  </si>
+  <si>
+    <t>Verify product sorting by price</t>
+  </si>
+  <si>
+    <t>GET /admin/products?sort=price&amp;order=asc</t>
+  </si>
+  <si>
+    <t>200 OK, products sorted ascending</t>
+  </si>
+  <si>
+    <t>Products sorted incorrectly</t>
+  </si>
+  <si>
+    <t>API-101</t>
+  </si>
+  <si>
+    <t>API-102</t>
+  </si>
+  <si>
+    <t>API-103</t>
+  </si>
+  <si>
+    <t>API-104</t>
+  </si>
+  <si>
+    <t>API-105</t>
+  </si>
+  <si>
+    <t>API-106</t>
+  </si>
+  <si>
+    <t>API-107</t>
+  </si>
+  <si>
+    <t>API-108</t>
+  </si>
+  <si>
+    <t>API-109</t>
+  </si>
+  <si>
+    <t>API-110</t>
+  </si>
+  <si>
+    <t>API-111</t>
+  </si>
+  <si>
+    <t>API-112</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1248,8 +1757,21 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1280,8 +1802,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1304,11 +1838,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1344,13 +1924,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1687,22 +2303,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6049C7D-8CCD-4133-8B86-7DF181C85485}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="73" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:G63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
+    <row r="1" spans="1:7" ht="28.8">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1725,57 +2342,57 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="90">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:7" ht="86.4">
+      <c r="A2" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>71</v>
+        <v>168</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="90">
-      <c r="A3" s="13"/>
+    <row r="3" spans="1:7" ht="57.6">
+      <c r="A3" s="16"/>
       <c r="B3" s="5" t="s">
-        <v>69</v>
+        <v>169</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>55</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60">
-      <c r="A4" s="13"/>
+    <row r="4" spans="1:7" ht="43.2">
+      <c r="A4" s="16"/>
       <c r="B4" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>55</v>
@@ -1790,101 +2407,101 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="150">
-      <c r="A5" s="13"/>
+    <row r="5" spans="1:7" ht="129.6">
+      <c r="A5" s="16"/>
       <c r="B5" s="5" t="s">
-        <v>65</v>
+        <v>171</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="150">
+    <row r="6" spans="1:7" ht="129.6">
       <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="75">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:7" ht="72">
+      <c r="A7" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>62</v>
+        <v>173</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="150">
-      <c r="A8" s="13"/>
+    <row r="8" spans="1:7" ht="129.6">
+      <c r="A8" s="16"/>
       <c r="B8" s="5" t="s">
-        <v>59</v>
+        <v>174</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="60">
-      <c r="A9" s="13"/>
+    <row r="9" spans="1:7" ht="43.2">
+      <c r="A9" s="16"/>
       <c r="B9" s="5" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>55</v>
@@ -1899,489 +2516,1593 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:7" ht="129.6">
+      <c r="A10" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="5" t="s">
+      <c r="B10" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="72">
+      <c r="A11" s="19"/>
+      <c r="B11" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="72">
+      <c r="A12" s="20"/>
+      <c r="B12" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="86.4">
+      <c r="A13" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" ht="75">
-      <c r="A13" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>82</v>
+      <c r="B13" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>133</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="120">
-      <c r="A14" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>111</v>
+    <row r="14" spans="1:7" ht="57.6">
+      <c r="A14" s="19"/>
+      <c r="B14" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="75">
-      <c r="A15" s="14"/>
-      <c r="B15" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>112</v>
+    <row r="15" spans="1:7" ht="86.4">
+      <c r="A15" s="19"/>
+      <c r="B15" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>89</v>
+        <v>140</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="75">
-      <c r="A16" s="14"/>
-      <c r="B16" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>113</v>
+    <row r="16" spans="1:7" ht="129.6">
+      <c r="A16" s="19"/>
+      <c r="B16" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="75">
-      <c r="A17" s="14"/>
-      <c r="B17" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>108</v>
+    <row r="17" spans="1:7" ht="86.4">
+      <c r="A17" s="20"/>
+      <c r="B17" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>147</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>92</v>
+        <v>166</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="135">
-      <c r="A18" s="14"/>
-      <c r="B18" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>115</v>
+    <row r="18" spans="1:7" ht="115.2">
+      <c r="A18" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="90">
-      <c r="A19" s="14"/>
-      <c r="B19" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>116</v>
+    <row r="19" spans="1:7" ht="57.6">
+      <c r="A19" s="19"/>
+      <c r="B19" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>154</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>101</v>
+        <v>167</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="75">
-      <c r="A20" s="14"/>
-      <c r="B20" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>117</v>
+    <row r="20" spans="1:7" ht="115.2">
+      <c r="A20" s="19"/>
+      <c r="B20" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>158</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>92</v>
+        <v>158</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="75">
-      <c r="A21" s="14"/>
-      <c r="B21" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>109</v>
+    <row r="21" spans="1:7" ht="129.6">
+      <c r="A21" s="19"/>
+      <c r="B21" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="75">
-      <c r="A22" s="14"/>
-      <c r="B22" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>110</v>
+    <row r="22" spans="1:7" ht="72">
+      <c r="A22" s="20"/>
+      <c r="B22" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:7" ht="72">
+      <c r="A23" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="100.8">
+      <c r="A24" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="72">
+      <c r="A25" s="17"/>
+      <c r="B25" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="72">
+      <c r="A26" s="17"/>
+      <c r="B26" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="72">
+      <c r="A27" s="17"/>
+      <c r="B27" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="129.6">
+      <c r="A28" s="17"/>
+      <c r="B28" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="86.4">
+      <c r="A29" s="17"/>
+      <c r="B29" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="72">
+      <c r="A30" s="17"/>
+      <c r="B30" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="72">
+      <c r="A31" s="17"/>
+      <c r="B31" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="72">
+      <c r="A32" s="17"/>
+      <c r="B32" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="5" t="s">
+      <c r="B33" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="G33" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="27"/>
+      <c r="B34" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="G34" s="25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="27"/>
+      <c r="B35" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="27"/>
+      <c r="B36" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="27"/>
+      <c r="B37" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="E37" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="G37" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="27"/>
+      <c r="B38" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="G38" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="27"/>
+      <c r="B39" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="27"/>
+      <c r="B40" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="G40" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="5" t="s">
+      <c r="B41" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="E41" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="G41" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="27"/>
+      <c r="B42" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="F42" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="G42" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="27"/>
+      <c r="B43" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="G43" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="27"/>
+      <c r="B44" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="E44" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="G44" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="27"/>
+      <c r="B45" s="23" t="s">
+        <v>268</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="D45" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="E45" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="F45" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="G45" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="27"/>
+      <c r="B46" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="E46" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="F46" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="G46" s="25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="27"/>
+      <c r="B47" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="C47" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="E47" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="F47" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="G47" s="25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="27"/>
+      <c r="B48" s="23" t="s">
+        <v>271</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>247</v>
+      </c>
+      <c r="G48" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="27"/>
+      <c r="B49" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="C49" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="D49" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="E49" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="F49" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="G49" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="27"/>
+      <c r="B50" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="C50" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="D50" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="E50" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="F50" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="G50" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="27"/>
+      <c r="B51" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="C51" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="D51" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="F51" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="G51" s="25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="27"/>
+      <c r="B52" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="C52" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="D52" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="E52" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="F52" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="G52" s="25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="5" t="s">
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" ht="105">
-      <c r="A27" s="13" t="s">
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+    </row>
+    <row r="56" spans="1:7" ht="100.8">
+      <c r="A56" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B56" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C56" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D56" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E56" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F56" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G56" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="75">
-      <c r="A28" s="13"/>
-      <c r="B28" s="5" t="s">
+    <row r="57" spans="1:7" ht="72">
+      <c r="A57" s="16"/>
+      <c r="B57" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C57" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D57" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E57" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F57" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G57" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="120">
-      <c r="A29" s="13"/>
-      <c r="B29" s="5" t="s">
+    <row r="58" spans="1:7" ht="115.2">
+      <c r="A58" s="16"/>
+      <c r="B58" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C58" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D58" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E58" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F58" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G58" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="348.75">
-      <c r="A30" s="13"/>
-      <c r="B30" s="5" t="s">
+    <row r="59" spans="1:7" ht="72">
+      <c r="A59" s="16"/>
+      <c r="B59" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C59" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D59" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E59" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F59" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G59" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="90">
-      <c r="A31" s="13" t="s">
+    <row r="60" spans="1:7" ht="72">
+      <c r="A60" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B60" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C60" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D60" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E60" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F60" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G60" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="145.5">
-      <c r="A32" s="13"/>
-      <c r="B32" s="5" t="s">
+    <row r="61" spans="1:7" ht="72">
+      <c r="A61" s="16"/>
+      <c r="B61" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C61" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D61" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E61" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F61" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G61" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="120">
-      <c r="A33" s="13"/>
-      <c r="B33" s="5" t="s">
+    <row r="62" spans="1:7" ht="115.2">
+      <c r="A62" s="16"/>
+      <c r="B62" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C62" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D62" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E62" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F62" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="G62" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="120">
-      <c r="A34" s="13"/>
-      <c r="B34" s="5" t="s">
+    <row r="63" spans="1:7" ht="72">
+      <c r="A63" s="16"/>
+      <c r="B63" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C63" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D63" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E63" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F63" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G63" s="11" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
+    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="A41:A52"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A14:A22"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A24:A32"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A22"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3918633E-C107-4F5B-8202-4A79DA60477C}">
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34:F38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="230.4">
+      <c r="A1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" ht="144">
+      <c r="A2" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" ht="100.8">
+      <c r="A3" s="22"/>
+      <c r="B3" s="7"/>
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" ht="302.39999999999998">
+      <c r="A4" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="115.2">
+      <c r="A5" s="22"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" t="s">
+        <v>163</v>
+      </c>
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" t="s">
+        <v>130</v>
+      </c>
+      <c r="F26" t="s">
+        <v>164</v>
+      </c>
+      <c r="G26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" t="s">
+        <v>136</v>
+      </c>
+      <c r="E29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" t="s">
+        <v>165</v>
+      </c>
+      <c r="G29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" t="s">
+        <v>139</v>
+      </c>
+      <c r="E30" t="s">
+        <v>140</v>
+      </c>
+      <c r="F30" t="s">
+        <v>140</v>
+      </c>
+      <c r="G30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" t="s">
+        <v>143</v>
+      </c>
+      <c r="E31" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" t="s">
+        <v>147</v>
+      </c>
+      <c r="F32" t="s">
+        <v>166</v>
+      </c>
+      <c r="G32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" t="s">
+        <v>149</v>
+      </c>
+      <c r="D34" t="s">
+        <v>150</v>
+      </c>
+      <c r="E34" t="s">
+        <v>151</v>
+      </c>
+      <c r="F34" t="s">
+        <v>151</v>
+      </c>
+      <c r="G34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>152</v>
+      </c>
+      <c r="C35" t="s">
+        <v>153</v>
+      </c>
+      <c r="D35" t="s">
+        <v>150</v>
+      </c>
+      <c r="E35" t="s">
+        <v>154</v>
+      </c>
+      <c r="F35" t="s">
+        <v>167</v>
+      </c>
+      <c r="G35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" t="s">
+        <v>155</v>
+      </c>
+      <c r="C36" t="s">
+        <v>156</v>
+      </c>
+      <c r="D36" t="s">
+        <v>157</v>
+      </c>
+      <c r="E36" t="s">
+        <v>158</v>
+      </c>
+      <c r="F36" t="s">
+        <v>158</v>
+      </c>
+      <c r="G36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37" t="s">
+        <v>142</v>
+      </c>
+      <c r="D37" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" t="s">
+        <v>161</v>
+      </c>
+      <c r="D38" t="s">
+        <v>162</v>
+      </c>
+      <c r="E38" t="s">
+        <v>140</v>
+      </c>
+      <c r="F38" t="s">
+        <v>140</v>
+      </c>
+      <c r="G38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2390,7 +4111,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A95317433F16A84E86C5BD170513CF32" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="465f8a72315053741d0bb1390d63bf9d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a1285e94-d8c3-4e5c-9ac5-21d2b8f33cfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="69b64cf170e112620a4780630ba75930" ns3:_="">
     <xsd:import namespace="a1285e94-d8c3-4e5c-9ac5-21d2b8f33cfd"/>
@@ -2540,23 +4261,13 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E13EB00-08F6-4D0A-BFA2-CC0D0ABB08B2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="a1285e94-d8c3-4e5c-9ac5-21d2b8f33cfd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B30151-59CC-41DF-A395-CB998ACFB3C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2564,7 +4275,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0719CEB4-C716-46CF-BE0B-B05697814749}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2580,4 +4291,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E13EB00-08F6-4D0A-BFA2-CC0D0ABB08B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="a1285e94-d8c3-4e5c-9ac5-21d2b8f33cfd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding plan and update APIs test
</commit_message>
<xml_diff>
--- a/API-Test-Cases.xlsx
+++ b/API-Test-Cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAPTOP\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEPI_GP\open-cart-demo-online-shopping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A3E85BE-1C51-4FD5-8288-922F3B317CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1265A29F-30C8-4D9C-8BFF-934C2B70310C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F506F1E7-1669-43D9-8551-1234B563D8BA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="287">
   <si>
     <r>
       <t xml:space="preserve">Valid </t>
@@ -1730,6 +1730,51 @@
   </si>
   <si>
     <t>API-112</t>
+  </si>
+  <si>
+    <t>Verify login with invalid email and password</t>
+  </si>
+  <si>
+    <t>Status Code: 404 Response Message: "User not found!"</t>
+  </si>
+  <si>
+    <t>Status Code = 404 Response Message = "User not found!"</t>
+  </si>
+  <si>
+    <t>POST https://automationexercise.com/api/createAccount</t>
+  </si>
+  <si>
+    <t>Verify that user can successfully create an account using valid form-data fields</t>
+  </si>
+  <si>
+    <t>name: Mahmoud email: Mahmoudtest@example.com password: 1222222 title: Eng birth_date: 5 birth_month: 12 birth_year: 1999 firstname: Mahmoud lastname: khaled company: TestCompany address1: Street 123 address2: Apartment 4 country: Canada zipcode: A1B2C3 state: Ontario city: Toronto mobile_number: 1234567890</t>
+  </si>
+  <si>
+    <r>
+      <t>Status Code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 201</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify that user account is successfully deleted when valid email and password are provided</t>
+  </si>
+  <si>
+    <t>email: Mahmoudtest@example.com password: 1222222</t>
+  </si>
+  <si>
+    <t>Status Code: 200,Response Message: "Account deleted!"</t>
+  </si>
+  <si>
+    <t>Status Code = 200,Response Message = "Account deleted!"</t>
   </si>
 </sst>
 </file>
@@ -1888,7 +1933,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1933,11 +1978,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1948,25 +2001,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2305,21 +2352,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6049C7D-8CCD-4133-8B86-7DF181C85485}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="73" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:G63"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="73" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.3984375" customWidth="1"/>
+    <col min="3" max="3" width="43.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.19921875" customWidth="1"/>
+    <col min="5" max="5" width="64.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.8">
+    <row r="1" spans="1:7" ht="27.6">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -2342,8 +2389,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="86.4">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:7" ht="69">
+      <c r="A2" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2365,8 +2412,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="57.6">
-      <c r="A3" s="16"/>
+    <row r="3" spans="1:7" ht="69">
+      <c r="A3" s="21"/>
       <c r="B3" s="5" t="s">
         <v>169</v>
       </c>
@@ -2386,8 +2433,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="43.2">
-      <c r="A4" s="16"/>
+    <row r="4" spans="1:7" ht="41.4">
+      <c r="A4" s="21"/>
       <c r="B4" s="5" t="s">
         <v>170</v>
       </c>
@@ -2407,8 +2454,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="129.6">
-      <c r="A5" s="16"/>
+    <row r="5" spans="1:7" ht="124.2">
+      <c r="A5" s="21"/>
       <c r="B5" s="5" t="s">
         <v>171</v>
       </c>
@@ -2428,7 +2475,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="129.6">
+    <row r="6" spans="1:7" ht="124.2">
       <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
@@ -2451,8 +2498,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="72">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:7" ht="69">
+      <c r="A7" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -2474,8 +2521,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="129.6">
-      <c r="A8" s="16"/>
+    <row r="8" spans="1:7" ht="124.2">
+      <c r="A8" s="21"/>
       <c r="B8" s="5" t="s">
         <v>174</v>
       </c>
@@ -2495,8 +2542,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="43.2">
-      <c r="A9" s="16"/>
+    <row r="9" spans="1:7" ht="41.4">
+      <c r="A9" s="21"/>
       <c r="B9" s="5" t="s">
         <v>175</v>
       </c>
@@ -2516,8 +2563,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="129.6">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:7" ht="124.2">
+      <c r="A10" s="22" t="s">
         <v>42</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -2539,8 +2586,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="72">
-      <c r="A11" s="19"/>
+    <row r="11" spans="1:7" ht="69">
+      <c r="A11" s="23"/>
       <c r="B11" s="5" t="s">
         <v>125</v>
       </c>
@@ -2560,8 +2607,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="72">
-      <c r="A12" s="20"/>
+    <row r="12" spans="1:7" ht="69">
+      <c r="A12" s="24"/>
       <c r="B12" s="5" t="s">
         <v>128</v>
       </c>
@@ -2581,8 +2628,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="86.4">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="1:7" ht="69">
+      <c r="A13" s="22" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -2604,8 +2651,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="57.6">
-      <c r="A14" s="19"/>
+    <row r="14" spans="1:7" ht="55.2">
+      <c r="A14" s="23"/>
       <c r="B14" s="5" t="s">
         <v>134</v>
       </c>
@@ -2625,8 +2672,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="86.4">
-      <c r="A15" s="19"/>
+    <row r="15" spans="1:7" ht="69">
+      <c r="A15" s="23"/>
       <c r="B15" s="5" t="s">
         <v>137</v>
       </c>
@@ -2646,8 +2693,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="129.6">
-      <c r="A16" s="19"/>
+    <row r="16" spans="1:7" ht="124.2">
+      <c r="A16" s="23"/>
       <c r="B16" s="5" t="s">
         <v>141</v>
       </c>
@@ -2667,8 +2714,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="86.4">
-      <c r="A17" s="20"/>
+    <row r="17" spans="1:7" ht="82.8">
+      <c r="A17" s="24"/>
       <c r="B17" s="5" t="s">
         <v>144</v>
       </c>
@@ -2688,8 +2735,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="115.2">
-      <c r="A18" s="18" t="s">
+    <row r="18" spans="1:7" ht="124.2">
+      <c r="A18" s="22" t="s">
         <v>44</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -2711,8 +2758,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="57.6">
-      <c r="A19" s="19"/>
+    <row r="19" spans="1:7" ht="55.2">
+      <c r="A19" s="23"/>
       <c r="B19" s="5" t="s">
         <v>152</v>
       </c>
@@ -2732,8 +2779,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="115.2">
-      <c r="A20" s="19"/>
+    <row r="20" spans="1:7" ht="124.2">
+      <c r="A20" s="23"/>
       <c r="B20" s="5" t="s">
         <v>155</v>
       </c>
@@ -2753,8 +2800,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="129.6">
-      <c r="A21" s="19"/>
+    <row r="21" spans="1:7" ht="124.2">
+      <c r="A21" s="23"/>
       <c r="B21" s="5" t="s">
         <v>159</v>
       </c>
@@ -2774,8 +2821,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="72">
-      <c r="A22" s="20"/>
+    <row r="22" spans="1:7" ht="69">
+      <c r="A22" s="24"/>
       <c r="B22" s="5" t="s">
         <v>160</v>
       </c>
@@ -2795,7 +2842,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="72">
+    <row r="23" spans="1:7" ht="69">
       <c r="A23" s="8" t="s">
         <v>45</v>
       </c>
@@ -2818,8 +2865,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="100.8">
-      <c r="A24" s="17" t="s">
+    <row r="24" spans="1:7" ht="110.4">
+      <c r="A24" s="27" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -2841,8 +2888,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="72">
-      <c r="A25" s="17"/>
+    <row r="25" spans="1:7" ht="69">
+      <c r="A25" s="27"/>
       <c r="B25" s="9" t="s">
         <v>79</v>
       </c>
@@ -2862,8 +2909,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="72">
-      <c r="A26" s="17"/>
+    <row r="26" spans="1:7" ht="69">
+      <c r="A26" s="27"/>
       <c r="B26" s="9" t="s">
         <v>82</v>
       </c>
@@ -2883,8 +2930,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="72">
-      <c r="A27" s="17"/>
+    <row r="27" spans="1:7" ht="69">
+      <c r="A27" s="27"/>
       <c r="B27" s="9" t="s">
         <v>85</v>
       </c>
@@ -2904,8 +2951,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="129.6">
-      <c r="A28" s="17"/>
+    <row r="28" spans="1:7" ht="124.2">
+      <c r="A28" s="27"/>
       <c r="B28" s="9" t="s">
         <v>87</v>
       </c>
@@ -2925,8 +2972,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="86.4">
-      <c r="A29" s="17"/>
+    <row r="29" spans="1:7" ht="82.8">
+      <c r="A29" s="27"/>
       <c r="B29" s="9" t="s">
         <v>90</v>
       </c>
@@ -2946,8 +2993,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="72">
-      <c r="A30" s="17"/>
+    <row r="30" spans="1:7" ht="69">
+      <c r="A30" s="27"/>
       <c r="B30" s="9" t="s">
         <v>94</v>
       </c>
@@ -2967,8 +3014,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="72">
-      <c r="A31" s="17"/>
+    <row r="31" spans="1:7" ht="69">
+      <c r="A31" s="27"/>
       <c r="B31" s="9" t="s">
         <v>96</v>
       </c>
@@ -2988,8 +3035,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="72">
-      <c r="A32" s="17"/>
+    <row r="32" spans="1:7" ht="69">
+      <c r="A32" s="27"/>
       <c r="B32" s="9" t="s">
         <v>98</v>
       </c>
@@ -3010,426 +3057,426 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="D33" s="23" t="s">
+      <c r="D33" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="E33" s="23" t="s">
+      <c r="E33" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="F33" s="23" t="s">
+      <c r="F33" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="G33" s="24" t="s">
+      <c r="G33" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="27"/>
-      <c r="B34" s="23" t="s">
+      <c r="A34" s="26"/>
+      <c r="B34" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="C34" s="23" t="s">
+      <c r="C34" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="D34" s="23" t="s">
+      <c r="D34" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="E34" s="23" t="s">
+      <c r="E34" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="F34" s="23" t="s">
+      <c r="F34" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="G34" s="25" t="s">
+      <c r="G34" s="18" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="27"/>
-      <c r="B35" s="23" t="s">
+      <c r="A35" s="26"/>
+      <c r="B35" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="D35" s="23" t="s">
+      <c r="D35" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E35" s="23" t="s">
+      <c r="E35" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="F35" s="23" t="s">
+      <c r="F35" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="G35" s="25" t="s">
+      <c r="G35" s="18" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="27"/>
-      <c r="B36" s="23" t="s">
+      <c r="A36" s="26"/>
+      <c r="B36" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="D36" s="23" t="s">
+      <c r="D36" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="E36" s="23" t="s">
+      <c r="E36" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="F36" s="23" t="s">
+      <c r="F36" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="G36" s="24" t="s">
+      <c r="G36" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="27"/>
-      <c r="B37" s="23" t="s">
+      <c r="A37" s="26"/>
+      <c r="B37" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="D37" s="23" t="s">
+      <c r="D37" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="E37" s="23" t="s">
+      <c r="E37" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="F37" s="23" t="s">
+      <c r="F37" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="G37" s="24" t="s">
+      <c r="G37" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="27"/>
-      <c r="B38" s="23" t="s">
+      <c r="A38" s="26"/>
+      <c r="B38" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="E38" s="23" t="s">
+      <c r="E38" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="F38" s="23" t="s">
+      <c r="F38" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="G38" s="24" t="s">
+      <c r="G38" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="27"/>
-      <c r="B39" s="23" t="s">
+      <c r="A39" s="26"/>
+      <c r="B39" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="C39" s="23" t="s">
+      <c r="C39" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="D39" s="23" t="s">
+      <c r="D39" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="E39" s="23" t="s">
+      <c r="E39" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="F39" s="23" t="s">
+      <c r="F39" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="G39" s="25" t="s">
+      <c r="G39" s="18" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="27"/>
-      <c r="B40" s="23" t="s">
+      <c r="A40" s="26"/>
+      <c r="B40" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="C40" s="23" t="s">
+      <c r="C40" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="D40" s="23" t="s">
+      <c r="D40" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="E40" s="23" t="s">
+      <c r="E40" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="F40" s="23" t="s">
+      <c r="F40" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="G40" s="24" t="s">
+      <c r="G40" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="26" t="s">
+      <c r="A41" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="C41" s="23" t="s">
+      <c r="C41" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="D41" s="23" t="s">
+      <c r="D41" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="E41" s="23" t="s">
+      <c r="E41" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="F41" s="23" t="s">
+      <c r="F41" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="G41" s="24" t="s">
+      <c r="G41" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="27"/>
-      <c r="B42" s="23" t="s">
+      <c r="A42" s="26"/>
+      <c r="B42" s="16" t="s">
         <v>265</v>
       </c>
-      <c r="C42" s="23" t="s">
+      <c r="C42" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="D42" s="23" t="s">
+      <c r="D42" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="E42" s="23" t="s">
+      <c r="E42" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="F42" s="23" t="s">
+      <c r="F42" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="G42" s="24" t="s">
+      <c r="G42" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="27"/>
-      <c r="B43" s="23" t="s">
+      <c r="A43" s="26"/>
+      <c r="B43" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="C43" s="23" t="s">
+      <c r="C43" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D43" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="E43" s="23" t="s">
+      <c r="E43" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="F43" s="23" t="s">
+      <c r="F43" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="G43" s="24" t="s">
+      <c r="G43" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="27"/>
-      <c r="B44" s="23" t="s">
+      <c r="A44" s="26"/>
+      <c r="B44" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="C44" s="23" t="s">
+      <c r="C44" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="D44" s="23" t="s">
+      <c r="D44" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="E44" s="23" t="s">
+      <c r="E44" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="F44" s="23" t="s">
+      <c r="F44" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="G44" s="24" t="s">
+      <c r="G44" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="27"/>
-      <c r="B45" s="23" t="s">
+      <c r="A45" s="26"/>
+      <c r="B45" s="16" t="s">
         <v>268</v>
       </c>
-      <c r="C45" s="23" t="s">
+      <c r="C45" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="D45" s="23" t="s">
+      <c r="D45" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="E45" s="23" t="s">
+      <c r="E45" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="F45" s="23" t="s">
+      <c r="F45" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="G45" s="24" t="s">
+      <c r="G45" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="27"/>
-      <c r="B46" s="23" t="s">
+      <c r="A46" s="26"/>
+      <c r="B46" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="C46" s="23" t="s">
+      <c r="C46" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="D46" s="23" t="s">
+      <c r="D46" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="E46" s="23" t="s">
+      <c r="E46" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="F46" s="23" t="s">
+      <c r="F46" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="G46" s="25" t="s">
+      <c r="G46" s="18" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="27"/>
-      <c r="B47" s="23" t="s">
+      <c r="A47" s="26"/>
+      <c r="B47" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="C47" s="23" t="s">
+      <c r="C47" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="D47" s="23" t="s">
+      <c r="D47" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="E47" s="23" t="s">
+      <c r="E47" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="F47" s="23" t="s">
+      <c r="F47" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="G47" s="25" t="s">
+      <c r="G47" s="18" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="27"/>
-      <c r="B48" s="23" t="s">
+      <c r="A48" s="26"/>
+      <c r="B48" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="C48" s="23" t="s">
+      <c r="C48" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="D48" s="23" t="s">
+      <c r="D48" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="E48" s="23" t="s">
+      <c r="E48" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="F48" s="23" t="s">
+      <c r="F48" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="G48" s="24" t="s">
+      <c r="G48" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="27"/>
-      <c r="B49" s="23" t="s">
+      <c r="A49" s="26"/>
+      <c r="B49" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="C49" s="23" t="s">
+      <c r="C49" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="D49" s="23" t="s">
+      <c r="D49" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="E49" s="23" t="s">
+      <c r="E49" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="F49" s="23" t="s">
+      <c r="F49" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="G49" s="24" t="s">
+      <c r="G49" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="27"/>
-      <c r="B50" s="23" t="s">
+      <c r="A50" s="26"/>
+      <c r="B50" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="C50" s="23" t="s">
+      <c r="C50" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="D50" s="23" t="s">
+      <c r="D50" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="E50" s="23" t="s">
+      <c r="E50" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="F50" s="23" t="s">
+      <c r="F50" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="G50" s="24" t="s">
+      <c r="G50" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="27"/>
-      <c r="B51" s="23" t="s">
+      <c r="A51" s="26"/>
+      <c r="B51" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="C51" s="23" t="s">
+      <c r="C51" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="D51" s="23" t="s">
+      <c r="D51" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="E51" s="23" t="s">
+      <c r="E51" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="F51" s="23" t="s">
+      <c r="F51" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="G51" s="25" t="s">
+      <c r="G51" s="18" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="27"/>
-      <c r="B52" s="23" t="s">
+      <c r="A52" s="26"/>
+      <c r="B52" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="C52" s="23" t="s">
+      <c r="C52" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="D52" s="23" t="s">
+      <c r="D52" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="E52" s="23" t="s">
+      <c r="E52" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="F52" s="23" t="s">
+      <c r="F52" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="G52" s="25" t="s">
+      <c r="G52" s="18" t="s">
         <v>184</v>
       </c>
     </row>
@@ -3437,37 +3484,73 @@
       <c r="A53" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
+      <c r="B53" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" t="s">
+        <v>276</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
+      <c r="B54" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54" t="s">
+        <v>280</v>
+      </c>
+      <c r="D54" t="s">
+        <v>281</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-    </row>
-    <row r="56" spans="1:7" ht="100.8">
-      <c r="A56" s="16" t="s">
+      <c r="B55" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" t="s">
+        <v>283</v>
+      </c>
+      <c r="D55" t="s">
+        <v>284</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="F55" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="G55" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="96.6">
+      <c r="A56" s="21" t="s">
         <v>51</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -3489,8 +3572,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="72">
-      <c r="A57" s="16"/>
+    <row r="57" spans="1:7" ht="69">
+      <c r="A57" s="21"/>
       <c r="B57" s="5" t="s">
         <v>4</v>
       </c>
@@ -3510,8 +3593,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="115.2">
-      <c r="A58" s="16"/>
+    <row r="58" spans="1:7" ht="110.4">
+      <c r="A58" s="21"/>
       <c r="B58" s="5" t="s">
         <v>6</v>
       </c>
@@ -3531,8 +3614,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="72">
-      <c r="A59" s="16"/>
+    <row r="59" spans="1:7" ht="69">
+      <c r="A59" s="21"/>
       <c r="B59" s="5" t="s">
         <v>7</v>
       </c>
@@ -3552,8 +3635,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="72">
-      <c r="A60" s="16" t="s">
+    <row r="60" spans="1:7" ht="69">
+      <c r="A60" s="21" t="s">
         <v>52</v>
       </c>
       <c r="B60" s="5" t="s">
@@ -3575,8 +3658,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="72">
-      <c r="A61" s="16"/>
+    <row r="61" spans="1:7" ht="69">
+      <c r="A61" s="21"/>
       <c r="B61" s="5" t="s">
         <v>4</v>
       </c>
@@ -3596,8 +3679,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="115.2">
-      <c r="A62" s="16"/>
+    <row r="62" spans="1:7" ht="96.6">
+      <c r="A62" s="21"/>
       <c r="B62" s="5" t="s">
         <v>6</v>
       </c>
@@ -3617,8 +3700,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="72">
-      <c r="A63" s="16"/>
+    <row r="63" spans="1:7" ht="69">
+      <c r="A63" s="21"/>
       <c r="B63" s="5" t="s">
         <v>7</v>
       </c>
@@ -3640,8 +3723,6 @@
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A33:A40"/>
-    <mergeCell ref="A41:A52"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A24:A32"/>
@@ -3650,6 +3731,8 @@
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="A41:A52"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3665,9 +3748,9 @@
       <selection activeCell="F34" sqref="F34:F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="230.4">
+    <row r="1" spans="1:7" ht="220.8">
       <c r="A1" s="5" t="s">
         <v>42</v>
       </c>
@@ -3684,8 +3767,8 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" ht="144">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:7" ht="138">
+      <c r="A2" s="28" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="7"/>
@@ -3701,8 +3784,8 @@
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="100.8">
-      <c r="A3" s="22"/>
+    <row r="3" spans="1:7" ht="96.6">
+      <c r="A3" s="29"/>
       <c r="B3" s="7"/>
       <c r="C3" t="s">
         <v>120</v>
@@ -3716,8 +3799,8 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" ht="302.39999999999998">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:7" ht="289.8">
+      <c r="A4" s="28" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="7"/>
@@ -3733,8 +3816,8 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="115.2">
-      <c r="A5" s="22"/>
+    <row r="5" spans="1:7" ht="110.4">
+      <c r="A5" s="29"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
         <v>117</v>

</xml_diff>